<commit_message>
Add mongoid-rspec gem for writing model rspec. Write the rspec for level and topic models.
</commit_message>
<xml_diff>
--- a/Learnings/Learnings.xlsx
+++ b/Learnings/Learnings.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Technology</t>
   </si>
@@ -28,6 +28,15 @@
   </si>
   <si>
     <t>Actual Code Affected</t>
+  </si>
+  <si>
+    <t>https://github.com/evansagge/mongoid-rspec</t>
+  </si>
+  <si>
+    <t>ROR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shulda matcher not supporting for writing rspec model. this model using mongodb databases. Use the gem called mongoid-rspec. </t>
   </si>
 </sst>
 </file>
@@ -383,7 +392,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -400,6 +409,17 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:4">

</xml_diff>